<commit_message>
Various fixes after laser cutting first pieces
</commit_message>
<xml_diff>
--- a/robot/cad/calculations.xlsx
+++ b/robot/cad/calculations.xlsx
@@ -163,12 +163,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -202,30 +203,34 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
-        <f aca="false">PI()/4</f>
-        <v>0.785398163397448</v>
+        <f aca="false">PI()/6</f>
+        <v>0.523598775598299</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">$A$1*COS(B3)</f>
-        <v>48.0832611206852</v>
+        <v>58.8897274573418</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">$A$1*SIN(B3)</f>
-        <v>48.0832611206852</v>
+        <v>34</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">SQRT(30*30+62*62)</f>
+        <v>68.8767014308903</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
-        <f aca="false">3*PI()/8</f>
-        <v>1.17809724509617</v>
+        <f aca="false">5*PI()/6</f>
+        <v>2.61799387799149</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">$A$1*COS(B4)</f>
-        <v>26.0224734008261</v>
+        <v>-58.8897274573418</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">$A$1*SIN(B4)</f>
-        <v>62.8238082107675</v>
+        <v>34</v>
       </c>
       <c r="I4" s="0" t="n">
         <f aca="false">SQRT(25.8^2+62.3^2)</f>
@@ -664,12 +669,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C31 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -690,12 +696,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C31 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>